<commit_message>
Changed some datasets and added new policy file.
</commit_message>
<xml_diff>
--- a/data/env_tax_gdp_per.xlsx
+++ b/data/env_tax_gdp_per.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\research_module\RM-project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\master_thesis\master_thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C2E3FD-BAF9-47E7-9799-34BA4C1EC5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73A8E7E-DFD8-4D87-90A5-FD55E9C17E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9830" yWindow="1280" windowWidth="8710" windowHeight="9140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="70">
   <si>
     <t>Environmental tax revenues [env_ac_tax__custom_14817925]</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>not available</t>
+  </si>
+  <si>
+    <t>Serbia</t>
   </si>
 </sst>
 </file>
@@ -306,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -329,11 +332,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB0B0B0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB0B0B0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -387,6 +401,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1259,10 +1276,10 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2327,6 +2344,38 @@
         <v>1.27</v>
       </c>
     </row>
+    <row r="34" spans="1:10" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="13">
+        <v>3.9</v>
+      </c>
+      <c r="C34" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D34" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E34" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F34" s="13">
+        <v>4.2</v>
+      </c>
+      <c r="G34" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H34" s="13">
+        <v>4</v>
+      </c>
+      <c r="I34" s="13">
+        <v>3.9</v>
+      </c>
+      <c r="J34" s="13">
+        <v>3.4</v>
+      </c>
+    </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>67</v>

</xml_diff>